<commit_message>
popMart: fix case cancel payment
</commit_message>
<xml_diff>
--- a/yodobashi.xlsx
+++ b/yodobashi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Hoai2005</t>
-  </si>
-  <si>
-    <t>https://www.yodobashi.com/product/100000001004518517</t>
   </si>
   <si>
     <t>https://www.yodobashi.com/product/100000001006404769, https://www.yodobashi.com/product/100000001004518517</t>
@@ -445,7 +442,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" activeCellId="1" sqref="A3 E7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -491,35 +488,20 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2" display="https://www.yodobashi.com/product/100000001006404769"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>